<commit_message>
Fixed some edge cases
</commit_message>
<xml_diff>
--- a/output_excel.xlsx
+++ b/output_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,6 +536,101 @@
         <v>1</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>2</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5499999999999999</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>0.5333333333333333</v>
+      </c>
+      <c r="D8" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>4</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>5</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>roll_roll</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Now getting all data points
</commit_message>
<xml_diff>
--- a/output_excel.xlsx
+++ b/output_excel.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,14 +485,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>_crawl</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.3666666666666667</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
       <c r="E3" t="n">
         <v>0.4</v>
@@ -504,14 +504,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>_crawl</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.3666666666666667</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="E4" t="n">
         <v>0.7</v>
@@ -523,14 +523,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>_crawl</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3666666666666667</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>0.9</v>
+        <v>0.7</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
@@ -542,14 +542,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>_crawl</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>1.2</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>1.3</v>
@@ -561,73 +561,244 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>roll_roll</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.5499999999999999</v>
+        <v>0.1571428571428572</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1.3</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>roll_roll</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.5333333333333333</v>
+        <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="E8" t="n">
-        <v>1.3</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>roll_crawl</t>
+          <t>roll_roll</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.55</v>
+        <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="E9" t="n">
-        <v>1.3</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
+        <v>2</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>roll_roll</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>roll_roll</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>roll_roll</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>3</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>0.2321428571428572</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>4</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>0.5928571428571427</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
         <v>5</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>5</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>5</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.6</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>5</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>roll_crawl</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>0.1428571428571428</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="E18" t="n">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>5</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>roll_roll</t>
         </is>
       </c>
-      <c r="C10" t="n">
-        <v>0.54</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
+      <c r="C19" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D19" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="E19" t="n">
         <v>1.3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
All current bugs have been fixed
</commit_message>
<xml_diff>
--- a/output_excel.xlsx
+++ b/output_excel.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -489,7 +489,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D3" t="n">
         <v>0.3</v>
@@ -508,7 +508,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D4" t="n">
         <v>0.6</v>
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D5" t="n">
         <v>0.9</v>
@@ -565,7 +565,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
@@ -584,7 +584,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D8" t="n">
         <v>0.1</v>
@@ -603,7 +603,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D9" t="n">
         <v>0.2</v>
@@ -622,7 +622,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D10" t="n">
         <v>0.3</v>
@@ -641,7 +641,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D11" t="n">
         <v>0.4</v>
@@ -660,7 +660,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D12" t="n">
         <v>0.5</v>
@@ -679,7 +679,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D13" t="n">
         <v>0.6</v>
@@ -698,7 +698,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D14" t="n">
         <v>0.7</v>
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D15" t="n">
         <v>0.8</v>
@@ -736,7 +736,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D16" t="n">
         <v>0.9</v>
@@ -755,7 +755,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -774,7 +774,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0.3666666666666667</v>
+        <v>0.55</v>
       </c>
       <c r="D18" t="n">
         <v>1.1</v>
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0.2321428571428572</v>
+        <v>0.5071428571428571</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.1428571428571428</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -869,7 +869,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.2285714285714286</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D23" t="n">
         <v>0.2</v>
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0.1833333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D24" t="n">
         <v>0.4</v>
@@ -907,7 +907,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>0.2285714285714286</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D25" t="n">
         <v>0.5</v>
@@ -926,7 +926,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0.1833333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D26" t="n">
         <v>0.7</v>
@@ -945,7 +945,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>0.2285714285714286</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D27" t="n">
         <v>0.8</v>
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>0.1833333333333333</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D28" t="n">
         <v>1</v>
@@ -983,7 +983,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0.2666666666666667</v>
+        <v>0.5333333333333333</v>
       </c>
       <c r="D29" t="n">
         <v>1.1</v>

</xml_diff>